<commit_message>
update demo last day
</commit_message>
<xml_diff>
--- a/doc/React_Memo.xlsx
+++ b/doc/React_Memo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\hachix\study\HACHIX_STUDY\React\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\talent5\Talent5PythonFlask\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABC219C-2E56-453F-B0E0-F18B9E157BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2471A2E-92FF-4792-BA06-25B9DCDE651B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23490" yWindow="5745" windowWidth="21600" windowHeight="11385" xr2:uid="{CF10ABB5-A789-4744-8845-DA7C6ED527D3}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{CF10ABB5-A789-4744-8845-DA7C6ED527D3}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicConcept" sheetId="1" r:id="rId1"/>
@@ -1472,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368C3106-17BD-4C77-8313-D8CFFFE11A58}">
   <dimension ref="A1:A106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
@@ -1510,7 +1510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7E9021-7902-413F-B5E4-3CA74928BFE5}">
   <dimension ref="B7:P55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A82" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>

</xml_diff>